<commit_message>
add recovered at home
</commit_message>
<xml_diff>
--- a/static/template_files/template-form-1.xlsx
+++ b/static/template_files/template-form-1.xlsx
@@ -20,45 +20,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Ngày</t>
   </si>
   <si>
-    <t xml:space="preserve">25/11/2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Số ca mới (PCR + test nhanh)</t>
   </si>
   <si>
-    <t xml:space="preserve">1582+916</t>
+    <t xml:space="preserve">1312+4142</t>
   </si>
   <si>
     <t xml:space="preserve">Tổng số ca (Đợt 4)</t>
   </si>
   <si>
-    <t xml:space="preserve">Xuất viện + Hồi phục tại khu cách ly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1148+648</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tổng số xuất viện + Hồi phục</t>
-  </si>
-  <si>
-    <t xml:space="preserve">273229+125726</t>
+    <t xml:space="preserve">Xuất viện + Hồi phục tại khu cách ly + Hồi phục tại nhà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1181+470+5597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng số xuất viện + Tổng hồi phục KCL + Tổng hồi phục tại nhà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">281867+130832+304554</t>
   </si>
   <si>
     <t xml:space="preserve">Số ca nhập viện + Đang điều trị</t>
   </si>
   <si>
-    <t xml:space="preserve">1582+14342</t>
+    <t xml:space="preserve">1262+13841</t>
   </si>
   <si>
     <t xml:space="preserve">Số ca nặng (thở máy xâm lấn + EMO) + Tử vong (tổng) + Tử vong (tỉnh khác)</t>
   </si>
   <si>
-    <t xml:space="preserve">357+10+59+12</t>
+    <t xml:space="preserve">408+13+68+7</t>
   </si>
   <si>
     <t xml:space="preserve">F0 đang theo dõi tại nhà</t>
@@ -70,13 +67,13 @@
     <t xml:space="preserve">Vaccine tiêm trong ngày (mũi 1 + mũi 2)</t>
   </si>
   <si>
-    <t xml:space="preserve">7165+233779</t>
+    <t xml:space="preserve">3095+13421</t>
   </si>
   <si>
     <t xml:space="preserve">Tổng số vaccine đã tiêm (mũi 1 + mũi 2)</t>
   </si>
   <si>
-    <t xml:space="preserve">7890985+6415954</t>
+    <t xml:space="preserve">7922727+6786683</t>
   </si>
 </sst>
 </file>
@@ -85,7 +82,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-42A]dd/mm/yyyy"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -113,31 +110,37 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,16 +177,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -192,6 +203,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -212,107 +227,110 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="14.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="n">
+        <v>44503</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="4" t="n">
+        <v>470512</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>457689</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="4" t="n">
+        <v>66874</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>60092</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="4" t="n">
+        <v>6072</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>6255</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>